<commit_message>
upload harness & input
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\東レ\toray\toray\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EC85D6-4A16-4AEB-912A-6746FBD94B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F655D5B-0D3C-449C-B5FF-472A20FDD1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SC-01" sheetId="27" r:id="rId1"/>
+    <sheet name="SC-12" sheetId="28" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
   <si>
     <t>name</t>
     <phoneticPr fontId="2"/>
@@ -227,6 +228,80 @@
   </si>
   <si>
     <t>3A1A-001435-0001</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ds_description</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ds_pattern</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>部長決裁</t>
+  </si>
+  <si>
+    <t>ds_discuss</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ds_copy</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1
+</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy-naoto.suzuki.g3@mail.toray,dummy-naoto.suzuki.g3@mail.toray
+</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy-takahiro.aoki.v8@mail.toray,dummy-takahiro.aoki.v8@mail.toray
+</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy-shinichi.imai.c2@mail.toray,dummy-shinichi.imai.c2@mail.toray
+</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest2
+</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest1testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttest
+</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy-naoto.suzuki.g3@mail.toray,dummy-takahiro.aoki.v8@mail.toray
+</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy-michihiro.akaki.t7@mail.toray
+</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy-naoto.suzuki.g3@mail.toray
+</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy-shinichi.imai.c2@mail.toray
+</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy-takahiro.aoki.v8@mail.toray
+</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -292,7 +367,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,6 +377,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,7 +403,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1"/>
@@ -341,6 +422,13 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -625,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA711085-9CB6-40E5-A86E-5A7BBC745BFD}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -869,4 +957,294 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF17EDD-8CC1-44DD-A9F0-61FEDC3783C6}">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <cols>
+    <col min="1" max="1" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.75" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="35.5" customWidth="1"/>
+    <col min="7" max="7" width="24" customWidth="1"/>
+    <col min="8" max="8" width="22.875" customWidth="1"/>
+    <col min="9" max="9" width="23.875" customWidth="1"/>
+    <col min="10" max="10" width="24.875" customWidth="1"/>
+    <col min="11" max="11" width="30.75" customWidth="1"/>
+    <col min="12" max="12" width="26.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="116.25" customHeight="1">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="108" customHeight="1">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" ht="135" customHeight="1">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4">
+        <v>9999</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="142.5" customHeight="1">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="180" customHeight="1">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="14"/>
+    </row>
+    <row r="7" spans="1:12" ht="147.75" customHeight="1">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="180.75" customHeight="1">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="162.75" customHeight="1">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="133.5" customHeight="1">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="139.5" customHeight="1">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="141" customHeight="1">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="121.5" customHeight="1">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{C04DAC65-BEFA-419A-86BF-A69D4762BCDC}"/>
+    <hyperlink ref="L2" r:id="rId2" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{309F15AD-52A3-4BE5-8EF4-34BA35D4B095}"/>
+    <hyperlink ref="K2" r:id="rId3" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{26A50205-BF5B-404B-B100-1D1637D20C9C}"/>
+    <hyperlink ref="G3" r:id="rId4" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{277C3B73-A213-4310-8D6D-4AD751F57D0A}"/>
+    <hyperlink ref="H3" r:id="rId5" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{461EF8DE-6257-492C-AA10-F3F6C4B7D0D3}"/>
+    <hyperlink ref="J4" r:id="rId6" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{E0F6462A-823C-426C-B374-9880394197D0}"/>
+    <hyperlink ref="K4" r:id="rId7" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{33BF89B5-7D28-4569-828D-E8C3FBB631F3}"/>
+    <hyperlink ref="G5" r:id="rId8" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{E8DBBDE1-B8FB-4114-ACEB-0ED884124140}"/>
+    <hyperlink ref="H5" r:id="rId9" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{5FC12360-1AFC-44CE-AF52-22C8BF75F6C9}"/>
+    <hyperlink ref="I5" r:id="rId10" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{C3A76C87-C620-4C5C-BD25-59AF5104937F}"/>
+    <hyperlink ref="K5" r:id="rId11" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{DE46C1FA-51BF-46E2-A408-767EE617B187}"/>
+    <hyperlink ref="G6" r:id="rId12" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{E34350ED-B5B5-4AD4-9C93-32FB34FB3A22}"/>
+    <hyperlink ref="I6" r:id="rId13" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{D599547C-BE9D-41C6-B88C-4C9E9FA0298C}"/>
+    <hyperlink ref="J6" r:id="rId14" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{F6C4EA90-7E8F-46AC-8BE1-065FC98A96E7}"/>
+    <hyperlink ref="G7" r:id="rId15" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{FB53E039-28EF-4E4A-8404-BA785B239582}"/>
+    <hyperlink ref="H7" r:id="rId16" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{C061606D-4ED4-433C-B912-2EA3A939AF17}"/>
+    <hyperlink ref="J5" r:id="rId17" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{E3D96F27-45D9-4636-8482-77D8B4FA36BE}"/>
+    <hyperlink ref="H6" r:id="rId18" display="dummy-naoto.suzuki.g3@mail.toray" xr:uid="{B98EB87E-70F4-4C5A-AA9C-FA2A1FF6B5F8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+</worksheet>
 </file>
</xml_diff>